<commit_message>
Regression for every category
</commit_message>
<xml_diff>
--- a/DEPRECATED/Data/job_vacancies_per_year.xlsx
+++ b/DEPRECATED/Data/job_vacancies_per_year.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unimi2013-my.sharepoint.com/personal/stefano_chiesa3_studenti_unimi_it/Documents/causal_inference_project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{66B0C0AA-382D-40BC-965B-53A44C7563AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64871A32-A43C-48B5-AA05-305558F38B8A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="106_{7DC878B7-FF23-4BEE-A17F-8E8F2236ABEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,45 +16,146 @@
     <sheet name="A" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="47">
   <si>
+    <t>Economic Activities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y2014  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">y2015  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">y2016  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">y2017  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">y2018  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">y2019  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">y2020  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">y2021  </t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>0.8</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mining and quarrying  </t>
   </si>
   <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Manufacturing  </t>
   </si>
   <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
     <t xml:space="preserve">Electricity, gas, steam and air conditioning supply  </t>
   </si>
   <si>
+    <t>0.4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Water supply sewerage, waste management and remediation activities  </t>
   </si>
   <si>
     <t xml:space="preserve">Construction  </t>
   </si>
   <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
     <t xml:space="preserve">Transportation and storage  </t>
   </si>
   <si>
     <t xml:space="preserve">Accommodation and food service activities  </t>
   </si>
   <si>
+    <t>2.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Information and communication  </t>
   </si>
   <si>
+    <t>2.3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Financial and insurance activities  </t>
   </si>
   <si>
     <t xml:space="preserve">Professional, scientific and technical activities  </t>
   </si>
   <si>
+    <t>1.9</t>
+  </si>
+  <si>
+    <t>2.9</t>
+  </si>
+  <si>
     <t xml:space="preserve">Administrative and support service activities  </t>
   </si>
   <si>
+    <t>1.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Education  </t>
   </si>
   <si>
@@ -64,103 +165,7 @@
     <t xml:space="preserve">Arts, entertainment and recreation  </t>
   </si>
   <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>Services</t>
-  </si>
-  <si>
-    <t>0.6</t>
-  </si>
-  <si>
-    <t>0.7</t>
-  </si>
-  <si>
-    <t>0.8</t>
-  </si>
-  <si>
-    <t>1.2</t>
-  </si>
-  <si>
-    <t>1.7</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>0.3</t>
-  </si>
-  <si>
-    <t>0.2</t>
-  </si>
-  <si>
-    <t>0.9</t>
-  </si>
-  <si>
-    <t>1.1</t>
-  </si>
-  <si>
-    <t>1.6</t>
-  </si>
-  <si>
-    <t>0.4</t>
-  </si>
-  <si>
-    <t>1.3</t>
-  </si>
-  <si>
-    <t>1.8</t>
-  </si>
-  <si>
-    <t>1.4</t>
-  </si>
-  <si>
-    <t>2.1</t>
-  </si>
-  <si>
-    <t>2.5</t>
-  </si>
-  <si>
-    <t>2.3</t>
-  </si>
-  <si>
-    <t>1.9</t>
-  </si>
-  <si>
-    <t>2.9</t>
-  </si>
-  <si>
-    <t>1.5</t>
-  </si>
-  <si>
     <t>2.2</t>
-  </si>
-  <si>
-    <t>Economic Activities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y2014  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">y2015  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">y2016  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">y2017  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">y2018  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">y2019  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">y2020  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">y2021  </t>
   </si>
 </sst>
 </file>
@@ -171,7 +176,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0#########################################################################################################################"/>
     <numFmt numFmtId="165" formatCode="0.0000000000000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -252,7 +257,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -268,7 +273,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -570,69 +575,69 @@
       <selection activeCell="B1" sqref="B1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="25" defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
@@ -641,431 +646,431 @@
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="29.1">
+      <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="43.5">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="I6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="G7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E8" s="2">
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H8" s="2">
         <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G9" s="2">
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="29.1">
       <c r="A10" s="3" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G10" s="2">
         <v>2</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="29.1">
       <c r="A11" s="3" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="H11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="29.1">
       <c r="A12" s="3" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="29.1">
       <c r="A13" s="3" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G13" s="2">
         <v>2</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="29.1">
       <c r="A14" s="3" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="3" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E15" s="2">
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I15" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="29.1">
       <c r="A16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="29.1">
+      <c r="A17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="I17" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="6"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>

</xml_diff>